<commit_message>
- remove context menu - widen a column width
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/tradeTemplate.xlsx
+++ b/src/main/webapp/WEB-INF/books/tradeTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD3391D7-A3A7-3C48-A81E-A653B08472DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865E5B0-0A30-EA46-B8D6-2B82197687A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38320" yWindow="3020" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,25 +201,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1" tint="0.14999847407452621"/>
-        <name val="Calibri"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
@@ -282,6 +263,25 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.14999847407452621"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -344,13 +344,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="0" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table4" displayName="Table4" ref="A1:D6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Salesperson" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sales" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Product" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Salesperson" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Sales" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -644,13 +644,14 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="7.796875" style="3" customWidth="1"/>
-    <col min="2" max="3" width="13.19921875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="13.19921875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.3984375" style="6" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
minor update trade template
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/books/tradeTemplate.xlsx
+++ b/src/main/webapp/WEB-INF/books/tradeTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11111"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/books/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7865E5B0-0A30-EA46-B8D6-2B82197687A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F1ABDA-B523-E641-B20C-B686FC979424}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38320" yWindow="3020" windowWidth="20740" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,18 +47,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -67,7 +67,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -76,7 +76,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -146,7 +146,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -181,17 +181,21 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已瀏覽過的超連結" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="超連結" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超連結" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -206,7 +210,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
@@ -647,15 +651,15 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.796875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="13.19921875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.59765625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" style="6" customWidth="1"/>
+    <col min="1" max="1" width="7.83203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="13.1640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" customHeight="1">
+    <row r="1" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -669,7 +673,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5" s="10"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6" s="10"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>

</xml_diff>